<commit_message>
Add complete product data to spreadsheet import/export
- Add ReorderPoint and OverstockThreshold fields to Product entity
- Update spreadsheet export to include Category Name, Supplier Name,
  Reorder Point, and Overstock Threshold columns
- Update spreadsheet import to link products by Category Name and
  Supplier Name when IDs are not provided, and import inventory fields
- Update ProductsPageViewModel to display actual ReorderPoint and
  OverstockThreshold values instead of hardcoded defaults
- Update modal view models to save and load the new inventory fields
- Update SampleCompanyData.xlsx with the new columns and sample data
- Remove unused CountryOfOrigin from ProductDisplayItem

This enables full round-trip export/import: users can export a company's
product data, then import it into a new company with all data preserved
including category and supplier relationships.
</commit_message>
<xml_diff>
--- a/ArgoBooks/Resources/SampleCompanyData.xlsx
+++ b/ArgoBooks/Resources/SampleCompanyData.xlsx
@@ -9160,7 +9160,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:N21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9206,7 +9206,27 @@
       </c>
       <c r="H1" t="inlineStr">
         <is>
+          <t>Category Name</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
           <t>Supplier ID</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>Supplier Name</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>Reorder Point</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>Overstock Threshold</t>
         </is>
       </c>
     </row>
@@ -9248,8 +9268,24 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
+          <t>Laptops</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
           <t>SUP-001</t>
         </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>Dell Technologies</t>
+        </is>
+      </c>
+      <c r="K2" t="n">
+        <v>10</v>
+      </c>
+      <c r="L2" t="n">
+        <v>100</v>
       </c>
     </row>
     <row r="3">
@@ -9290,8 +9326,24 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
+          <t>Laptops</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
           <t>SUP-001</t>
         </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Dell Technologies</t>
+        </is>
+      </c>
+      <c r="K3" t="n">
+        <v>10</v>
+      </c>
+      <c r="L3" t="n">
+        <v>100</v>
       </c>
     </row>
     <row r="4">
@@ -9332,8 +9384,24 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
+          <t>Laptops</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
           <t>SUP-007</t>
         </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Lenovo</t>
+        </is>
+      </c>
+      <c r="K4" t="n">
+        <v>10</v>
+      </c>
+      <c r="L4" t="n">
+        <v>100</v>
       </c>
     </row>
     <row r="5">
@@ -9374,8 +9442,24 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
+          <t>Desktops</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
           <t>SUP-001</t>
         </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Dell Technologies</t>
+        </is>
+      </c>
+      <c r="K5" t="n">
+        <v>10</v>
+      </c>
+      <c r="L5" t="n">
+        <v>100</v>
       </c>
     </row>
     <row r="6">
@@ -9416,8 +9500,24 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
+          <t>Desktops</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
           <t>SUP-001</t>
         </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>Dell Technologies</t>
+        </is>
+      </c>
+      <c r="K6" t="n">
+        <v>10</v>
+      </c>
+      <c r="L6" t="n">
+        <v>100</v>
       </c>
     </row>
     <row r="7">
@@ -9458,8 +9558,24 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
+          <t>Monitors</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
           <t>SUP-001</t>
         </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>Dell Technologies</t>
+        </is>
+      </c>
+      <c r="K7" t="n">
+        <v>10</v>
+      </c>
+      <c r="L7" t="n">
+        <v>100</v>
       </c>
     </row>
     <row r="8">
@@ -9500,8 +9616,24 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
+          <t>Monitors</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
           <t>SUP-001</t>
         </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>Dell Technologies</t>
+        </is>
+      </c>
+      <c r="K8" t="n">
+        <v>10</v>
+      </c>
+      <c r="L8" t="n">
+        <v>100</v>
       </c>
     </row>
     <row r="9">
@@ -9542,8 +9674,24 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
+          <t>Networking</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
           <t>SUP-004</t>
         </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>Cisco Systems</t>
+        </is>
+      </c>
+      <c r="K9" t="n">
+        <v>10</v>
+      </c>
+      <c r="L9" t="n">
+        <v>100</v>
       </c>
     </row>
     <row r="10">
@@ -9584,8 +9732,24 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
+          <t>Networking</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
           <t>SUP-004</t>
         </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>Cisco Systems</t>
+        </is>
+      </c>
+      <c r="K10" t="n">
+        <v>10</v>
+      </c>
+      <c r="L10" t="n">
+        <v>100</v>
       </c>
     </row>
     <row r="11">
@@ -9626,8 +9790,24 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
+          <t>Networking</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
           <t>SUP-002</t>
         </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>Ingram Micro</t>
+        </is>
+      </c>
+      <c r="K11" t="n">
+        <v>10</v>
+      </c>
+      <c r="L11" t="n">
+        <v>100</v>
       </c>
     </row>
     <row r="12">
@@ -9668,8 +9848,24 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
+          <t>Peripherals</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
           <t>SUP-002</t>
         </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>Ingram Micro</t>
+        </is>
+      </c>
+      <c r="K12" t="n">
+        <v>10</v>
+      </c>
+      <c r="L12" t="n">
+        <v>100</v>
       </c>
     </row>
     <row r="13">
@@ -9710,8 +9906,24 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
+          <t>Peripherals</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
           <t>SUP-002</t>
         </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>Ingram Micro</t>
+        </is>
+      </c>
+      <c r="K13" t="n">
+        <v>10</v>
+      </c>
+      <c r="L13" t="n">
+        <v>100</v>
       </c>
     </row>
     <row r="14">
@@ -9752,8 +9964,24 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
+          <t>Peripherals</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
           <t>SUP-002</t>
         </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>Ingram Micro</t>
+        </is>
+      </c>
+      <c r="K14" t="n">
+        <v>10</v>
+      </c>
+      <c r="L14" t="n">
+        <v>100</v>
       </c>
     </row>
     <row r="15">
@@ -9794,8 +10022,24 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
+          <t>Software</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
           <t>SUP-005</t>
         </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>Microsoft Corporation</t>
+        </is>
+      </c>
+      <c r="K15" t="n">
+        <v>10</v>
+      </c>
+      <c r="L15" t="n">
+        <v>100</v>
       </c>
     </row>
     <row r="16">
@@ -9836,8 +10080,24 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
+          <t>Software</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
           <t>SUP-003</t>
         </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>Tech Data Corporation</t>
+        </is>
+      </c>
+      <c r="K16" t="n">
+        <v>10</v>
+      </c>
+      <c r="L16" t="n">
+        <v>100</v>
       </c>
     </row>
     <row r="17">
@@ -9876,6 +10136,18 @@
           <t>CAT-SAL-009</t>
         </is>
       </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>Support Contracts</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr"/>
+      <c r="K17" t="n">
+        <v>0</v>
+      </c>
+      <c r="L17" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -9913,6 +10185,18 @@
           <t>CAT-SAL-009</t>
         </is>
       </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>Support Contracts</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr"/>
+      <c r="K18" t="n">
+        <v>0</v>
+      </c>
+      <c r="L18" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -9950,6 +10234,18 @@
           <t>CAT-SAL-010</t>
         </is>
       </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>Consulting</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr"/>
+      <c r="K19" t="n">
+        <v>0</v>
+      </c>
+      <c r="L19" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -9987,6 +10283,18 @@
           <t>CAT-SAL-010</t>
         </is>
       </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>Consulting</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr"/>
+      <c r="K20" t="n">
+        <v>0</v>
+      </c>
+      <c r="L20" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -10023,6 +10331,18 @@
         <is>
           <t>CAT-SAL-010</t>
         </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>Consulting</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr"/>
+      <c r="K21" t="n">
+        <v>0</v>
+      </c>
+      <c r="L21" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improve purchase order modal and add line items support
- Add space before asterisks on required fields for consistency
- Restyle line items section to match expenses/revenue modals
- Add purchase order line items to sample company data
- Add import/export support for purchase order line items

https://claude.ai/code/session_01UzMCiUaj9wG5AA52LYnEaW
</commit_message>
<xml_diff>
--- a/ArgoBooks/Resources/SampleCompanyData.xlsx
+++ b/ArgoBooks/Resources/SampleCompanyData.xlsx
@@ -24,6 +24,7 @@
     <sheet name="Rental Inventory" sheetId="15" state="visible" r:id="rId15"/>
     <sheet name="Rental Records" sheetId="16" state="visible" r:id="rId16"/>
     <sheet name="Recurring Invoices" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet name="Purchase Order Line Items" sheetId="18" state="visible" r:id="rId18"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -33,7 +34,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -41,13 +42,22 @@
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00ADD8E6"/>
+        <bgColor rgb="00ADD8E6"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -62,8 +72,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -8051,6 +8064,479 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="8" customWidth="1" min="1" max="1"/>
+    <col width="12" customWidth="1" min="2" max="2"/>
+    <col width="10" customWidth="1" min="3" max="3"/>
+    <col width="11" customWidth="1" min="4" max="4"/>
+    <col width="19" customWidth="1" min="5" max="5"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>PO ID</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Product ID</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Quantity</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Unit Cost</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Quantity Received</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>PO-001</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>PRD-001</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>5</v>
+      </c>
+      <c r="D2" t="n">
+        <v>899</v>
+      </c>
+      <c r="E2" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>PO-001</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>PRD-004</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>5</v>
+      </c>
+      <c r="D3" t="n">
+        <v>699</v>
+      </c>
+      <c r="E3" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>PO-001</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>PRD-007</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>11</v>
+      </c>
+      <c r="D4" t="n">
+        <v>149</v>
+      </c>
+      <c r="E4" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>PO-002</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>PRD-002</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>3</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1349</v>
+      </c>
+      <c r="E5" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>PO-002</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>PRD-006</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>6</v>
+      </c>
+      <c r="D6" t="n">
+        <v>349</v>
+      </c>
+      <c r="E6" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>PO-003</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>PRD-008</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>2</v>
+      </c>
+      <c r="D7" t="n">
+        <v>1195</v>
+      </c>
+      <c r="E7" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>PO-003</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>PRD-009</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" t="n">
+        <v>1515</v>
+      </c>
+      <c r="E8" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>PO-004</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>PRD-002</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>4</v>
+      </c>
+      <c r="D9" t="n">
+        <v>1349</v>
+      </c>
+      <c r="E9" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>PO-004</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>PRD-001</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>3</v>
+      </c>
+      <c r="D10" t="n">
+        <v>899</v>
+      </c>
+      <c r="E10" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>PO-004</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>PRD-007</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>4</v>
+      </c>
+      <c r="D11" t="n">
+        <v>149</v>
+      </c>
+      <c r="E11" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>PO-005</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>PRD-005</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>3</v>
+      </c>
+      <c r="D12" t="n">
+        <v>1999</v>
+      </c>
+      <c r="E12" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>PO-005</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>PRD-004</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>2</v>
+      </c>
+      <c r="D13" t="n">
+        <v>699</v>
+      </c>
+      <c r="E13" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>PO-005</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>PRD-007</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>3</v>
+      </c>
+      <c r="D14" t="n">
+        <v>149</v>
+      </c>
+      <c r="E14" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>PO-006</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>PRD-001</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>4</v>
+      </c>
+      <c r="D15" t="n">
+        <v>899</v>
+      </c>
+      <c r="E15" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>PO-006</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>PRD-006</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>5</v>
+      </c>
+      <c r="D16" t="n">
+        <v>349</v>
+      </c>
+      <c r="E16" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>PO-006</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>PRD-007</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>3</v>
+      </c>
+      <c r="D17" t="n">
+        <v>149</v>
+      </c>
+      <c r="E17" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>PO-007</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>PRD-002</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>3</v>
+      </c>
+      <c r="D18" t="n">
+        <v>1349</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>PO-007</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>PRD-004</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>2</v>
+      </c>
+      <c r="D19" t="n">
+        <v>699</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>PO-007</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>PRD-006</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>3</v>
+      </c>
+      <c r="D20" t="n">
+        <v>349</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>PO-008</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>PRD-003</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>6</v>
+      </c>
+      <c r="D21" t="n">
+        <v>849</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
@@ -9160,7 +9646,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N21"/>
+  <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10141,7 +10627,6 @@
           <t>Support Contracts</t>
         </is>
       </c>
-      <c r="J17" t="inlineStr"/>
       <c r="K17" t="n">
         <v>0</v>
       </c>
@@ -10190,7 +10675,6 @@
           <t>Support Contracts</t>
         </is>
       </c>
-      <c r="J18" t="inlineStr"/>
       <c r="K18" t="n">
         <v>0</v>
       </c>
@@ -10239,7 +10723,6 @@
           <t>Consulting</t>
         </is>
       </c>
-      <c r="J19" t="inlineStr"/>
       <c r="K19" t="n">
         <v>0</v>
       </c>
@@ -10288,7 +10771,6 @@
           <t>Consulting</t>
         </is>
       </c>
-      <c r="J20" t="inlineStr"/>
       <c r="K20" t="n">
         <v>0</v>
       </c>
@@ -10337,7 +10819,6 @@
           <t>Consulting</t>
         </is>
       </c>
-      <c r="J21" t="inlineStr"/>
       <c r="K21" t="n">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Fix sample company data with proper expense products and categories
- Add 20 expense-type products (PRD-021 to PRD-040) with proper
  categories (Inventory Purchases, Office Supplies, Software
  Subscriptions, Professional Services, Marketing)
- Rename inventory expense products with "(Inventory)" suffix to
  differentiate from revenue products with same base name
- Update Expenses sheet to reference the correct expense product names
- Fix product name mismatches (removed quantity info like "10 units")
- Bump sample company version to 2.1.1 to force recreation

This fixes:
- Products showing "-" for Category, Supplier, Reorder, Overstock
- Categories showing "0" for Products/Services count
- All expense transactions now properly link to expense products

https://claude.ai/code/session_01By47KV9FqVf5HwxAAydRBq
</commit_message>
<xml_diff>
--- a/ArgoBooks/Resources/SampleCompanyData.xlsx
+++ b/ArgoBooks/Resources/SampleCompanyData.xlsx
@@ -4912,7 +4912,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Dell Latitude 5540 Laptop (10 units)</t>
+          <t>Dell Latitude 5540 Laptop (Inventory)</t>
         </is>
       </c>
       <c r="E2" t="n">
@@ -4953,7 +4953,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Dell OptiPlex 7010 Desktop (8 units)</t>
+          <t>Dell OptiPlex 7010 Desktop (Inventory)</t>
         </is>
       </c>
       <c r="E3" t="n">
@@ -4994,7 +4994,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Dell UltraSharp U2722D Monitor (10 units)</t>
+          <t>Dell UltraSharp U2722D Monitor (Inventory)</t>
         </is>
       </c>
       <c r="E4" t="n">
@@ -5035,7 +5035,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Lenovo ThinkPad T14 (6 units)</t>
+          <t>Lenovo ThinkPad T14 (Inventory)</t>
         </is>
       </c>
       <c r="E5" t="n">
@@ -5076,7 +5076,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Cisco Meraki MX68 Firewall (3 units)</t>
+          <t>Cisco Meraki MX68 Firewall (Inventory)</t>
         </is>
       </c>
       <c r="E6" t="n">
@@ -5117,7 +5117,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Dell P2422H Monitor (12 units)</t>
+          <t>Dell P2422H Monitor (Inventory)</t>
         </is>
       </c>
       <c r="E7" t="n">
@@ -5158,7 +5158,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Dell Precision 3660 Workstation (4 units)</t>
+          <t>Dell Precision 3660 Workstation (Inventory)</t>
         </is>
       </c>
       <c r="E8" t="n">
@@ -5199,7 +5199,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Cisco Catalyst 1000-24T Switch (4 units)</t>
+          <t>Cisco Catalyst 1000-24T Switch (Inventory)</t>
         </is>
       </c>
       <c r="E9" t="n">
@@ -5240,7 +5240,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Dell Latitude 7440 Laptop (5 units)</t>
+          <t>Dell Latitude 7440 Laptop (Inventory)</t>
         </is>
       </c>
       <c r="E10" t="n">
@@ -5322,7 +5322,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Dell Latitude 5540 Laptop (8 units)</t>
+          <t>Dell Latitude 5540 Laptop (Inventory)</t>
         </is>
       </c>
       <c r="E12" t="n">
@@ -5363,7 +5363,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Dell OptiPlex 7010 Desktop (6 units)</t>
+          <t>Dell OptiPlex 7010 Desktop (Inventory)</t>
         </is>
       </c>
       <c r="E13" t="n">
@@ -5404,7 +5404,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Ubiquiti UniFi Access Point (15 units)</t>
+          <t>Ubiquiti UniFi Access Point (Inventory)</t>
         </is>
       </c>
       <c r="E14" t="n">
@@ -5445,7 +5445,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Dell Latitude 5540 Laptop (6 units)</t>
+          <t>Dell Latitude 5540 Laptop (Inventory)</t>
         </is>
       </c>
       <c r="E15" t="n">
@@ -5486,7 +5486,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Dell Latitude 7440 Laptop (4 units)</t>
+          <t>Dell Latitude 7440 Laptop (Inventory)</t>
         </is>
       </c>
       <c r="E16" t="n">
@@ -5527,7 +5527,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Dell Precision 3660 Workstation (3 units)</t>
+          <t>Dell Precision 3660 Workstation (Inventory)</t>
         </is>
       </c>
       <c r="E17" t="n">
@@ -9646,7 +9646,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L21"/>
+  <dimension ref="A1:L41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10823,6 +10823,1136 @@
         <v>0</v>
       </c>
       <c r="L21" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>PRD-021</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Dell Latitude 5540 Laptop (Inventory)</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Expenses</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Product</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>EXP-DELL-LAT5540</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Purchase of Dell Latitude 5540 laptops for inventory</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>CAT-PUR-001</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>Inventory Purchases</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>SUP-001</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>Dell Technologies</t>
+        </is>
+      </c>
+      <c r="K22" t="n">
+        <v>5</v>
+      </c>
+      <c r="L22" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>PRD-022</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Dell Latitude 7440 Laptop (Inventory)</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Expenses</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Product</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>EXP-DELL-LAT7440</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Purchase of Dell Latitude 7440 laptops for inventory</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>CAT-PUR-001</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>Inventory Purchases</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>SUP-001</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>Dell Technologies</t>
+        </is>
+      </c>
+      <c r="K23" t="n">
+        <v>5</v>
+      </c>
+      <c r="L23" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>PRD-023</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Dell OptiPlex 7010 Desktop (Inventory)</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Expenses</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Product</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>EXP-DELL-OPT7010</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>Purchase of Dell OptiPlex desktops for inventory</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>CAT-PUR-001</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>Inventory Purchases</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>SUP-001</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>Dell Technologies</t>
+        </is>
+      </c>
+      <c r="K24" t="n">
+        <v>5</v>
+      </c>
+      <c r="L24" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>PRD-024</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Dell Precision 3660 Workstation (Inventory)</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Expenses</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Product</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>EXP-DELL-PREC3660</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>Purchase of Dell Precision workstations for inventory</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>CAT-PUR-001</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>Inventory Purchases</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>SUP-001</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>Dell Technologies</t>
+        </is>
+      </c>
+      <c r="K25" t="n">
+        <v>3</v>
+      </c>
+      <c r="L25" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>PRD-025</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Dell UltraSharp U2722D Monitor (Inventory)</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Expenses</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Product</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>EXP-DELL-U2722D</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>Purchase of Dell UltraSharp monitors for inventory</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>CAT-PUR-001</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>Inventory Purchases</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>SUP-001</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>Dell Technologies</t>
+        </is>
+      </c>
+      <c r="K26" t="n">
+        <v>5</v>
+      </c>
+      <c r="L26" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>PRD-026</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Dell P2422H Monitor (Inventory)</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Expenses</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Product</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>EXP-DELL-P2422H</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>Purchase of Dell P2422H monitors for inventory</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>CAT-PUR-001</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>Inventory Purchases</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>SUP-001</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>Dell Technologies</t>
+        </is>
+      </c>
+      <c r="K27" t="n">
+        <v>5</v>
+      </c>
+      <c r="L27" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>PRD-027</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Lenovo ThinkPad T14 (Inventory)</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Expenses</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Product</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>EXP-LEN-T14</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>Purchase of Lenovo ThinkPad laptops for inventory</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>CAT-PUR-001</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>Inventory Purchases</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>SUP-007</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>Lenovo</t>
+        </is>
+      </c>
+      <c r="K28" t="n">
+        <v>5</v>
+      </c>
+      <c r="L28" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>PRD-028</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Cisco Meraki MX68 Firewall (Inventory)</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Expenses</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Product</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>EXP-CISCO-MX68</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>Purchase of Cisco Meraki firewalls for inventory</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>CAT-PUR-001</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>Inventory Purchases</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>SUP-004</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>Cisco Systems</t>
+        </is>
+      </c>
+      <c r="K29" t="n">
+        <v>2</v>
+      </c>
+      <c r="L29" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>PRD-029</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Cisco Catalyst 1000-24T Switch (Inventory)</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Expenses</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Product</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>EXP-CISCO-CAT1000</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>Purchase of Cisco switches for inventory</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>CAT-PUR-001</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>Inventory Purchases</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>SUP-004</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>Cisco Systems</t>
+        </is>
+      </c>
+      <c r="K30" t="n">
+        <v>2</v>
+      </c>
+      <c r="L30" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>PRD-030</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Ubiquiti UniFi Access Point (Inventory)</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Expenses</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Product</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>EXP-UBNT-UAP</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>Purchase of Ubiquiti access points for inventory</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>CAT-PUR-001</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>Inventory Purchases</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>SUP-002</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>Ingram Micro</t>
+        </is>
+      </c>
+      <c r="K31" t="n">
+        <v>5</v>
+      </c>
+      <c r="L31" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>PRD-031</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Office Supplies - Q1</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Expenses</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Product</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>EXP-OFF-Q1</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>Q1 office supplies purchase</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>CAT-PUR-002</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>Office Supplies</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>SUP-002</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>Ingram Micro</t>
+        </is>
+      </c>
+      <c r="K32" t="n">
+        <v>0</v>
+      </c>
+      <c r="L32" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>PRD-032</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Office Supplies - Q2</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Expenses</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Product</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>EXP-OFF-Q2</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>Q2 office supplies purchase</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>CAT-PUR-002</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>Office Supplies</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>SUP-002</t>
+        </is>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>Ingram Micro</t>
+        </is>
+      </c>
+      <c r="K33" t="n">
+        <v>0</v>
+      </c>
+      <c r="L33" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>PRD-033</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Office Supplies - Q3</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Expenses</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>Product</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>EXP-OFF-Q3</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>Q3 office supplies purchase</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>CAT-PUR-002</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>Office Supplies</t>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>SUP-002</t>
+        </is>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>Ingram Micro</t>
+        </is>
+      </c>
+      <c r="K34" t="n">
+        <v>0</v>
+      </c>
+      <c r="L34" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>PRD-034</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Office Supplies - Q4</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Expenses</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>Product</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>EXP-OFF-Q4</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>Q4 office supplies purchase</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>CAT-PUR-002</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>Office Supplies</t>
+        </is>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>SUP-002</t>
+        </is>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>Ingram Micro</t>
+        </is>
+      </c>
+      <c r="K35" t="n">
+        <v>0</v>
+      </c>
+      <c r="L35" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>PRD-035</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Logitech Peripherals Bundle</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Expenses</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>Product</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>EXP-LOG-BUNDLE</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>Logitech keyboard, mouse, and webcam bundle</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>CAT-PUR-001</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>Inventory Purchases</t>
+        </is>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>SUP-002</t>
+        </is>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>Ingram Micro</t>
+        </is>
+      </c>
+      <c r="K36" t="n">
+        <v>5</v>
+      </c>
+      <c r="L36" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>PRD-036</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Adobe Creative Cloud (8 licenses)</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Expenses</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>Service</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>EXP-ADOBE-CC8</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>Adobe Creative Cloud subscription (8 licenses)</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>CAT-PUR-003</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>Software Subscriptions</t>
+        </is>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>SUP-005</t>
+        </is>
+      </c>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>CDW Corporation</t>
+        </is>
+      </c>
+      <c r="K37" t="n">
+        <v>0</v>
+      </c>
+      <c r="L37" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>PRD-037</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Microsoft 365 Business (40 licenses)</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Expenses</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>Service</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>EXP-MS365-40</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>Microsoft 365 Business subscription (40 licenses)</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>CAT-PUR-003</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>Software Subscriptions</t>
+        </is>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>SUP-003</t>
+        </is>
+      </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>Tech Data Corporation</t>
+        </is>
+      </c>
+      <c r="K38" t="n">
+        <v>0</v>
+      </c>
+      <c r="L38" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>PRD-038</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Professional Development Training</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Expenses</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>Service</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>EXP-TRAIN</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>Employee professional development and training</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>CAT-PUR-004</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>Professional Services</t>
+        </is>
+      </c>
+      <c r="K39" t="n">
+        <v>0</v>
+      </c>
+      <c r="L39" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>PRD-039</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Marketing - Fall Campaign</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Expenses</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>Service</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>EXP-MKT-FALL</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>Fall marketing campaign expenses</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>CAT-PUR-005</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>Marketing</t>
+        </is>
+      </c>
+      <c r="K40" t="n">
+        <v>0</v>
+      </c>
+      <c r="L40" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>PRD-040</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Marketing - Spring Campaign</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Expenses</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>Service</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>EXP-MKT-SPRING</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>Spring marketing campaign expenses</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>CAT-PUR-005</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>Marketing</t>
+        </is>
+      </c>
+      <c r="K41" t="n">
+        <v>0</v>
+      </c>
+      <c r="L41" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix sample returns data and lost/damaged modal overlay
- Add both Expense (3) and Customer (4) returns to sample data so
  returns table shows data in both tabs
- Fix LostDamagedPage modals to use ModalOverlay control for proper
  full-screen overlay coverage
- Bump sample company version to 2.2.1 to trigger recreation

https://claude.ai/code/session_01By47KV9FqVf5HwxAAydRBq
</commit_message>
<xml_diff>
--- a/ArgoBooks/Resources/SampleCompanyData.xlsx
+++ b/ArgoBooks/Resources/SampleCompanyData.xlsx
@@ -8745,7 +8745,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8823,35 +8823,35 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Customer</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>CUS-009</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr"/>
+          <t>Expense</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>SUP-006</t>
+        </is>
+      </c>
       <c r="E2" t="inlineStr">
         <is>
           <t>Cisco Meraki MX68 Firewall</t>
         </is>
       </c>
       <c r="F2" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G2" s="2" t="n">
-        <v>46039.89542372725</v>
+        <v>45995.90923776707</v>
       </c>
       <c r="H2" t="n">
-        <v>276.53</v>
+        <v>411.1</v>
       </c>
       <c r="I2" t="n">
         <v>0</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>Not as described</t>
+          <t>Defective</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
@@ -8869,31 +8869,31 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Customer</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>CUS-004</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr"/>
+          <t>Expense</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>SUP-002</t>
+        </is>
+      </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Cisco Catalyst 1000-24T Switch</t>
+          <t>Microsoft 365 Business Premium</t>
         </is>
       </c>
       <c r="F3" t="n">
         <v>1</v>
       </c>
       <c r="G3" s="2" t="n">
-        <v>46044.89542372725</v>
+        <v>46009.90923776707</v>
       </c>
       <c r="H3" t="n">
-        <v>245.73</v>
+        <v>446.24</v>
       </c>
       <c r="I3" t="n">
-        <v>24.57</v>
+        <v>0</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
@@ -8915,35 +8915,35 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Customer</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>CUS-007</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr"/>
+          <t>Expense</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>SUP-007</t>
+        </is>
+      </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Cisco Meraki MX68 Firewall</t>
+          <t>Cisco Catalyst 1000-24T Switch</t>
         </is>
       </c>
       <c r="F4" t="n">
         <v>3</v>
       </c>
       <c r="G4" s="2" t="n">
-        <v>46032.89542372725</v>
+        <v>46022.90923776707</v>
       </c>
       <c r="H4" t="n">
-        <v>61.21</v>
+        <v>170.61</v>
       </c>
       <c r="I4" t="n">
         <v>0</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>Damaged in shipping</t>
+          <t>Changed mind</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
@@ -8966,30 +8966,30 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>CUS-004</t>
+          <t>CUS-007</t>
         </is>
       </c>
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Adobe Creative Cloud</t>
+          <t>Dell OptiPlex 7010 Desktop</t>
         </is>
       </c>
       <c r="F5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G5" s="2" t="n">
-        <v>46000.89542372725</v>
+        <v>45999.90923776707</v>
       </c>
       <c r="H5" t="n">
-        <v>172.17</v>
+        <v>207.8</v>
       </c>
       <c r="I5" t="n">
-        <v>17.22</v>
+        <v>0</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>Defective</t>
+          <t>Changed mind</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
@@ -9012,30 +9012,30 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>CUS-005</t>
+          <t>CUS-006</t>
         </is>
       </c>
       <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Server Setup &amp; Configuration</t>
+          <t>Ubiquiti UniFi Access Point</t>
         </is>
       </c>
       <c r="F6" t="n">
         <v>2</v>
       </c>
       <c r="G6" s="2" t="n">
-        <v>46031.89542372725</v>
+        <v>46016.90923776707</v>
       </c>
       <c r="H6" t="n">
-        <v>112.95</v>
+        <v>248.64</v>
       </c>
       <c r="I6" t="n">
-        <v>11.3</v>
+        <v>0</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>Wrong item</t>
+          <t>Changed mind</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
@@ -9044,6 +9044,98 @@
         </is>
       </c>
       <c r="L6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>RET-006</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Customer</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>CUS-007</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Monthly IT Support Contract</t>
+        </is>
+      </c>
+      <c r="F7" t="n">
+        <v>2</v>
+      </c>
+      <c r="G7" s="2" t="n">
+        <v>46048.90923776707</v>
+      </c>
+      <c r="H7" t="n">
+        <v>272.62</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>Changed mind</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>RET-007</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Customer</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>CUS-008</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Monthly IT Support Contract</t>
+        </is>
+      </c>
+      <c r="F8" t="n">
+        <v>1</v>
+      </c>
+      <c r="G8" s="2" t="n">
+        <v>46028.90923776707</v>
+      </c>
+      <c r="H8" t="n">
+        <v>98.38</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>Not as described</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -9658,7 +9750,7 @@
         </is>
       </c>
       <c r="E2" s="2" t="n">
-        <v>46005.89542372725</v>
+        <v>46005.89542372686</v>
       </c>
       <c r="F2" t="n">
         <v>411.58</v>
@@ -9668,7 +9760,6 @@
           <t>No</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -9690,7 +9781,7 @@
         </is>
       </c>
       <c r="E3" s="2" t="n">
-        <v>46047.89542372725</v>
+        <v>46047.89542372686</v>
       </c>
       <c r="F3" t="n">
         <v>276.89</v>
@@ -9700,7 +9791,6 @@
           <t>Yes</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -9722,7 +9812,7 @@
         </is>
       </c>
       <c r="E4" s="2" t="n">
-        <v>46045.89542372725</v>
+        <v>46045.89542372686</v>
       </c>
       <c r="F4" t="n">
         <v>376.86</v>
@@ -9732,7 +9822,6 @@
           <t>No</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -9754,7 +9843,7 @@
         </is>
       </c>
       <c r="E5" s="2" t="n">
-        <v>46037.89542372725</v>
+        <v>46037.89542372686</v>
       </c>
       <c r="F5" t="n">
         <v>425.15</v>
@@ -9764,7 +9853,6 @@
           <t>No</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Add diverse countries to sample company data
Diversify customer and supplier countries in the sample data spreadsheet
to include various western countries (US, Canada, UK, Australia, Germany,
France, Ireland, Netherlands, New Zealand, Spain, Italy, Switzerland, Japan)
instead of all being USA.

https://claude.ai/code/session_01FL1LGuen8SqRYDWPsXGkDf
</commit_message>
<xml_diff>
--- a/ArgoBooks/Resources/SampleCompanyData.xlsx
+++ b/ArgoBooks/Resources/SampleCompanyData.xlsx
@@ -571,7 +571,7 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>USA</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
@@ -636,7 +636,7 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>USA</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
@@ -701,7 +701,7 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>USA</t>
+          <t>United Kingdom</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
@@ -766,7 +766,7 @@
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>USA</t>
+          <t>Australia</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
@@ -826,7 +826,7 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>USA</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
@@ -891,7 +891,7 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>USA</t>
+          <t>France</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
@@ -956,7 +956,7 @@
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>USA</t>
+          <t>Ireland</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
@@ -1021,7 +1021,7 @@
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>USA</t>
+          <t>Netherlands</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
@@ -1086,7 +1086,7 @@
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>USA</t>
+          <t>New Zealand</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
@@ -1146,7 +1146,7 @@
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>USA</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
@@ -1211,7 +1211,7 @@
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>USA</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
@@ -1276,7 +1276,7 @@
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>USA</t>
+          <t>United Kingdom</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
@@ -1341,7 +1341,7 @@
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>USA</t>
+          <t>Spain</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
@@ -1406,7 +1406,7 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>USA</t>
+          <t>Italy</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
@@ -1471,7 +1471,7 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>USA</t>
+          <t>Switzerland</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
@@ -8826,7 +8826,6 @@
           <t>Expense</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr">
         <is>
           <t>SUP-006</t>
@@ -8841,7 +8840,7 @@
         <v>5</v>
       </c>
       <c r="G2" s="2" t="n">
-        <v>45995.90923776707</v>
+        <v>45995.9092377662</v>
       </c>
       <c r="H2" t="n">
         <v>411.1</v>
@@ -8859,7 +8858,6 @@
           <t>Completed</t>
         </is>
       </c>
-      <c r="L2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -8872,7 +8870,6 @@
           <t>Expense</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr">
         <is>
           <t>SUP-002</t>
@@ -8887,7 +8884,7 @@
         <v>1</v>
       </c>
       <c r="G3" s="2" t="n">
-        <v>46009.90923776707</v>
+        <v>46009.9092377662</v>
       </c>
       <c r="H3" t="n">
         <v>446.24</v>
@@ -8905,7 +8902,6 @@
           <t>Completed</t>
         </is>
       </c>
-      <c r="L3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -8918,7 +8914,6 @@
           <t>Expense</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr">
         <is>
           <t>SUP-007</t>
@@ -8933,7 +8928,7 @@
         <v>3</v>
       </c>
       <c r="G4" s="2" t="n">
-        <v>46022.90923776707</v>
+        <v>46022.9092377662</v>
       </c>
       <c r="H4" t="n">
         <v>170.61</v>
@@ -8951,7 +8946,6 @@
           <t>Completed</t>
         </is>
       </c>
-      <c r="L4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -8969,7 +8963,6 @@
           <t>CUS-007</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr">
         <is>
           <t>Dell OptiPlex 7010 Desktop</t>
@@ -8979,7 +8972,7 @@
         <v>1</v>
       </c>
       <c r="G5" s="2" t="n">
-        <v>45999.90923776707</v>
+        <v>45999.9092377662</v>
       </c>
       <c r="H5" t="n">
         <v>207.8</v>
@@ -8997,7 +8990,6 @@
           <t>Completed</t>
         </is>
       </c>
-      <c r="L5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -9015,7 +9007,6 @@
           <t>CUS-006</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr">
         <is>
           <t>Ubiquiti UniFi Access Point</t>
@@ -9025,7 +9016,7 @@
         <v>2</v>
       </c>
       <c r="G6" s="2" t="n">
-        <v>46016.90923776707</v>
+        <v>46016.9092377662</v>
       </c>
       <c r="H6" t="n">
         <v>248.64</v>
@@ -9043,7 +9034,6 @@
           <t>Completed</t>
         </is>
       </c>
-      <c r="L6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -9061,7 +9051,6 @@
           <t>CUS-007</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr">
         <is>
           <t>Monthly IT Support Contract</t>
@@ -9071,7 +9060,7 @@
         <v>2</v>
       </c>
       <c r="G7" s="2" t="n">
-        <v>46048.90923776707</v>
+        <v>46048.9092377662</v>
       </c>
       <c r="H7" t="n">
         <v>272.62</v>
@@ -9089,7 +9078,6 @@
           <t>Completed</t>
         </is>
       </c>
-      <c r="L7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -9107,7 +9095,6 @@
           <t>CUS-008</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr">
         <is>
           <t>Monthly IT Support Contract</t>
@@ -9117,7 +9104,7 @@
         <v>1</v>
       </c>
       <c r="G8" s="2" t="n">
-        <v>46028.90923776707</v>
+        <v>46028.9092377662</v>
       </c>
       <c r="H8" t="n">
         <v>98.38</v>
@@ -9135,7 +9122,6 @@
           <t>Completed</t>
         </is>
       </c>
-      <c r="L8" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -9261,7 +9247,7 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>USA</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
@@ -9318,7 +9304,7 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>USA</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
@@ -9375,7 +9361,7 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>USA</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
@@ -9432,7 +9418,7 @@
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>USA</t>
+          <t>United Kingdom</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
@@ -9489,7 +9475,7 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>USA</t>
+          <t>Australia</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
@@ -9546,7 +9532,7 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>USA</t>
+          <t>France</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
@@ -9603,7 +9589,7 @@
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>USA</t>
+          <t>Netherlands</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
@@ -9660,7 +9646,7 @@
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>USA</t>
+          <t>Japan</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">

</xml_diff>

<commit_message>
Update rental modals and tables, improve country distribution
- Update sample company spreadsheet with more diverse country distribution
  (less USA, more Canada and other western countries)
- Change rental item modal from Item Name to Product SearchBox
- Remove Supplier field from rental item modals (derived from product)
- Add ProductId field to RentalItem model
- Remove Supplier column from rental inventory table
- Remove Accountant column from rental records table

https://claude.ai/code/session_01FL1LGuen8SqRYDWPsXGkDf
</commit_message>
<xml_diff>
--- a/ArgoBooks/Resources/SampleCompanyData.xlsx
+++ b/ArgoBooks/Resources/SampleCompanyData.xlsx
@@ -571,7 +571,7 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
@@ -636,7 +636,7 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>United Kingdom</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
@@ -701,7 +701,7 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>United Kingdom</t>
+          <t>Australia</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
@@ -766,7 +766,7 @@
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>Australia</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
@@ -9247,7 +9247,7 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
@@ -9304,7 +9304,7 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>United Kingdom</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
@@ -9418,7 +9418,7 @@
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>United Kingdom</t>
+          <t>Australia</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
@@ -9475,7 +9475,7 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>Australia</t>
+          <t>France</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
@@ -9532,7 +9532,7 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>France</t>
+          <t>Netherlands</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
@@ -9589,7 +9589,7 @@
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>Netherlands</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">

</xml_diff>

<commit_message>
Add undo/redo for mark as returned/lost and fix sample data
- Add undo/redo support for marking transactions as returned
- Add undo/redo support for marking transactions as lost/damaged
- Fix product names in Lost Damaged sheet in sample data
- Fix sample data linking for returns and losses

https://claude.ai/code/session_01MWAWYe2N3J94cmvPrVMSiA
</commit_message>
<xml_diff>
--- a/ArgoBooks/Resources/SampleCompanyData.xlsx
+++ b/ArgoBooks/Resources/SampleCompanyData.xlsx
@@ -5069,7 +5069,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Dell Latitude 5540 Laptop (Inventory)</t>
+          <t>Dell Latitude 5540 Laptop</t>
         </is>
       </c>
       <c r="E2" t="n">
@@ -5113,7 +5113,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Dell OptiPlex 7010 Desktop (Inventory)</t>
+          <t>Dell OptiPlex 7010 Desktop</t>
         </is>
       </c>
       <c r="E3" t="n">
@@ -5157,7 +5157,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Dell UltraSharp U2722D Monitor (Inventory)</t>
+          <t>Dell UltraSharp U2722D Monitor</t>
         </is>
       </c>
       <c r="E4" t="n">
@@ -5198,7 +5198,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Lenovo ThinkPad T14 (Inventory)</t>
+          <t>Lenovo ThinkPad T14</t>
         </is>
       </c>
       <c r="E5" t="n">
@@ -5242,7 +5242,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Cisco Meraki MX68 Firewall (Inventory)</t>
+          <t>Cisco Meraki MX68 Firewall</t>
         </is>
       </c>
       <c r="E6" t="n">
@@ -5286,7 +5286,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Dell P2422H Monitor (Inventory)</t>
+          <t>Dell P2422H Monitor</t>
         </is>
       </c>
       <c r="E7" t="n">
@@ -5330,7 +5330,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Dell Precision 3660 Workstation (Inventory)</t>
+          <t>Dell Precision 3660 Workstation</t>
         </is>
       </c>
       <c r="E8" t="n">
@@ -5371,7 +5371,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Cisco Catalyst 1000-24T Switch (Inventory)</t>
+          <t>Cisco Catalyst 1000-24T Switch</t>
         </is>
       </c>
       <c r="E9" t="n">
@@ -5412,7 +5412,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Dell Latitude 7440 Laptop (Inventory)</t>
+          <t>Dell Latitude 7440 Laptop</t>
         </is>
       </c>
       <c r="E10" t="n">
@@ -5497,7 +5497,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Dell Latitude 5540 Laptop (Inventory)</t>
+          <t>Dell Latitude 5540 Laptop</t>
         </is>
       </c>
       <c r="E12" t="n">
@@ -5541,7 +5541,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Dell OptiPlex 7010 Desktop (Inventory)</t>
+          <t>Dell OptiPlex 7010 Desktop</t>
         </is>
       </c>
       <c r="E13" t="n">
@@ -5582,7 +5582,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Ubiquiti UniFi Access Point (Inventory)</t>
+          <t>Ubiquiti UniFi Access Point</t>
         </is>
       </c>
       <c r="E14" t="n">
@@ -5623,7 +5623,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Dell Latitude 5540 Laptop (Inventory)</t>
+          <t>Dell Latitude 5540 Laptop</t>
         </is>
       </c>
       <c r="E15" t="n">
@@ -5664,7 +5664,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Dell Latitude 7440 Laptop (Inventory)</t>
+          <t>Dell Latitude 7440 Laptop</t>
         </is>
       </c>
       <c r="E16" t="n">
@@ -5708,7 +5708,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Dell Precision 3660 Workstation (Inventory)</t>
+          <t>Dell Precision 3660 Workstation</t>
         </is>
       </c>
       <c r="E17" t="n">
@@ -8745,7 +8745,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8761,55 +8761,60 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
+          <t>Original Transaction ID</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
           <t>Return Type</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>Customer ID</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>Supplier ID</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>Product</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>Quantity</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>Return Date</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>Refund Amount</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>Restocking Fee</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>Reason</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>Status</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>Notes</t>
         </is>
@@ -8823,37 +8828,42 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>PUR-2025-005</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
           <t>Expense</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>SUP-006</t>
-        </is>
-      </c>
       <c r="E2" t="inlineStr">
         <is>
+          <t>SUP-004</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
           <t>Cisco Meraki MX68 Firewall</t>
         </is>
       </c>
-      <c r="F2" t="n">
-        <v>5</v>
-      </c>
-      <c r="G2" s="2" t="n">
-        <v>45995.9092377662</v>
-      </c>
-      <c r="H2" t="n">
+      <c r="G2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2" s="2" t="n">
+        <v>46025.88398792824</v>
+      </c>
+      <c r="I2" t="n">
         <v>411.1</v>
       </c>
-      <c r="I2" t="n">
+      <c r="J2" t="n">
         <v>0</v>
       </c>
-      <c r="J2" t="inlineStr">
+      <c r="K2" t="inlineStr">
         <is>
           <t>Defective</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr">
+      <c r="L2" t="inlineStr">
         <is>
           <t>Completed</t>
         </is>
@@ -8867,37 +8877,42 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
+          <t>PUR-2025-008</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
           <t>Expense</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>SUP-002</t>
-        </is>
-      </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Microsoft 365 Business Premium</t>
-        </is>
-      </c>
-      <c r="F3" t="n">
+          <t>SUP-004</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Cisco Catalyst 1000-24T Switch</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
         <v>1</v>
       </c>
-      <c r="G3" s="2" t="n">
-        <v>46009.9092377662</v>
-      </c>
-      <c r="H3" t="n">
-        <v>446.24</v>
+      <c r="H3" s="2" t="n">
+        <v>46035.88398792824</v>
       </c>
       <c r="I3" t="n">
+        <v>170.61</v>
+      </c>
+      <c r="J3" t="n">
         <v>0</v>
       </c>
-      <c r="J3" t="inlineStr">
+      <c r="K3" t="inlineStr">
         <is>
           <t>Not as described</t>
         </is>
       </c>
-      <c r="K3" t="inlineStr">
+      <c r="L3" t="inlineStr">
         <is>
           <t>Completed</t>
         </is>
@@ -8911,37 +8926,42 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
+          <t>PUR-2025-010</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
           <t>Expense</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>SUP-007</t>
-        </is>
-      </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Cisco Catalyst 1000-24T Switch</t>
-        </is>
-      </c>
-      <c r="F4" t="n">
-        <v>3</v>
-      </c>
-      <c r="G4" s="2" t="n">
-        <v>46022.9092377662</v>
-      </c>
-      <c r="H4" t="n">
-        <v>170.61</v>
+          <t>SUP-002</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Logitech Peripherals Bundle</t>
+        </is>
+      </c>
+      <c r="G4" t="n">
+        <v>1</v>
+      </c>
+      <c r="H4" s="2" t="n">
+        <v>46045.88398792824</v>
       </c>
       <c r="I4" t="n">
+        <v>89.98999999999999</v>
+      </c>
+      <c r="J4" t="n">
         <v>0</v>
       </c>
-      <c r="J4" t="inlineStr">
+      <c r="K4" t="inlineStr">
         <is>
           <t>Changed mind</t>
         </is>
       </c>
-      <c r="K4" t="inlineStr">
+      <c r="L4" t="inlineStr">
         <is>
           <t>Completed</t>
         </is>
@@ -8955,37 +8975,42 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
+          <t>SAL-2025-013</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
           <t>Customer</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>CUS-007</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Dell OptiPlex 7010 Desktop</t>
-        </is>
-      </c>
-      <c r="F5" t="n">
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>CUS-006</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Lenovo ThinkPad T14</t>
+        </is>
+      </c>
+      <c r="G5" t="n">
         <v>1</v>
       </c>
-      <c r="G5" s="2" t="n">
-        <v>45999.9092377662</v>
-      </c>
-      <c r="H5" t="n">
-        <v>207.8</v>
+      <c r="H5" s="2" t="n">
+        <v>46030.88398792824</v>
       </c>
       <c r="I5" t="n">
-        <v>0</v>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>Changed mind</t>
-        </is>
+        <v>1299</v>
+      </c>
+      <c r="J5" t="n">
+        <v>50</v>
       </c>
       <c r="K5" t="inlineStr">
+        <is>
+          <t>Defective</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
         <is>
           <t>Completed</t>
         </is>
@@ -8999,125 +9024,42 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
+          <t>SAL-2025-006</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
           <t>Customer</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>CUS-006</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Ubiquiti UniFi Access Point</t>
-        </is>
-      </c>
-      <c r="F6" t="n">
-        <v>2</v>
-      </c>
-      <c r="G6" s="2" t="n">
-        <v>46016.9092377662</v>
-      </c>
-      <c r="H6" t="n">
-        <v>248.64</v>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>CUS-004</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Dell OptiPlex 7010 Desktop</t>
+        </is>
+      </c>
+      <c r="G6" t="n">
+        <v>1</v>
+      </c>
+      <c r="H6" s="2" t="n">
+        <v>46040.88398792824</v>
       </c>
       <c r="I6" t="n">
+        <v>899</v>
+      </c>
+      <c r="J6" t="n">
         <v>0</v>
       </c>
-      <c r="J6" t="inlineStr">
+      <c r="K6" t="inlineStr">
         <is>
           <t>Changed mind</t>
         </is>
       </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>Completed</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>RET-006</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Customer</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>CUS-007</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>Monthly IT Support Contract</t>
-        </is>
-      </c>
-      <c r="F7" t="n">
-        <v>2</v>
-      </c>
-      <c r="G7" s="2" t="n">
-        <v>46048.9092377662</v>
-      </c>
-      <c r="H7" t="n">
-        <v>272.62</v>
-      </c>
-      <c r="I7" t="n">
-        <v>0</v>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>Changed mind</t>
-        </is>
-      </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>Completed</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>RET-007</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Customer</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>CUS-008</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>Monthly IT Support Contract</t>
-        </is>
-      </c>
-      <c r="F8" t="n">
-        <v>1</v>
-      </c>
-      <c r="G8" s="2" t="n">
-        <v>46028.9092377662</v>
-      </c>
-      <c r="H8" t="n">
-        <v>98.38</v>
-      </c>
-      <c r="I8" t="n">
-        <v>0</v>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>Not as described</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
+      <c r="L6" t="inlineStr">
         <is>
           <t>Completed</t>
         </is>
@@ -9666,7 +9608,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9682,35 +9624,40 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
+          <t>Inventory Item ID</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
           <t>Product</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>Quantity</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>Reason</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>Date Discovered</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>Value Lost</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>Insurance Claim</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>Notes</t>
         </is>
@@ -9724,26 +9671,36 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Cisco Catalyst 1000-24T Switch</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>5</v>
-      </c>
-      <c r="D2" t="inlineStr">
+          <t>PUR-2025-001</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Dell Latitude 5540 Laptop</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" t="inlineStr">
         <is>
           <t>Damaged</t>
         </is>
       </c>
-      <c r="E2" s="2" t="n">
-        <v>46005.89542372686</v>
-      </c>
-      <c r="F2" t="n">
-        <v>411.58</v>
-      </c>
-      <c r="G2" t="inlineStr">
+      <c r="F2" s="2" t="n">
+        <v>46010.88398792824</v>
+      </c>
+      <c r="G2" t="n">
+        <v>1199</v>
+      </c>
+      <c r="H2" t="inlineStr">
         <is>
           <t>No</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Screen cracked during transport</t>
         </is>
       </c>
     </row>
@@ -9755,26 +9712,36 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
+          <t>PUR-2025-004</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
           <t>Lenovo ThinkPad T14</t>
         </is>
       </c>
-      <c r="C3" t="n">
-        <v>5</v>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Expired</t>
-        </is>
-      </c>
-      <c r="E3" s="2" t="n">
-        <v>46047.89542372686</v>
-      </c>
-      <c r="F3" t="n">
-        <v>276.89</v>
-      </c>
-      <c r="G3" t="inlineStr">
+      <c r="D3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Lost</t>
+        </is>
+      </c>
+      <c r="F3" s="2" t="n">
+        <v>46020.88398792824</v>
+      </c>
+      <c r="G3" t="n">
+        <v>1299</v>
+      </c>
+      <c r="H3" t="inlineStr">
         <is>
           <t>Yes</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Missing from inventory</t>
         </is>
       </c>
     </row>
@@ -9786,57 +9753,36 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Dell Latitude 5540 Laptop</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>5</v>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Other</t>
-        </is>
-      </c>
-      <c r="E4" s="2" t="n">
-        <v>46045.89542372686</v>
-      </c>
-      <c r="F4" t="n">
-        <v>376.86</v>
-      </c>
-      <c r="G4" t="inlineStr">
+          <t>PUR-2025-003</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Dell UltraSharp U2722D Monitor</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Damaged</t>
+        </is>
+      </c>
+      <c r="F4" s="2" t="n">
+        <v>46027.88398792824</v>
+      </c>
+      <c r="G4" t="n">
+        <v>449</v>
+      </c>
+      <c r="H4" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>LOST-004</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Cisco Meraki MX68 Firewall</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>2</v>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Damaged</t>
-        </is>
-      </c>
-      <c r="E5" s="2" t="n">
-        <v>46037.89542372686</v>
-      </c>
-      <c r="F5" t="n">
-        <v>425.15</v>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>No</t>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Water damage</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add rental record, inventory, and dashboard improvements
Dashboard:
- Make active rentals list clickable with full-row hover effect

Rental records:
- Add 'Mark as Paid' checkbox to rental process return modal
- Add 'Mark as Paid' action button for returned unpaid records
- Move dates before line items in rental record modals

Rental inventory:
- Hide rent-out button when unavailable
- Fix edit modal product dropdown
- Include both Rental and Revenue products in dropdown
- Add Rental products to sample spreadsheet

https://claude.ai/code/session_017LsMJ6vkduGspbXE2K4DeD
</commit_message>
<xml_diff>
--- a/ArgoBooks/Resources/SampleCompanyData.xlsx
+++ b/ArgoBooks/Resources/SampleCompanyData.xlsx
@@ -7415,7 +7415,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7474,6 +7474,11 @@
           <t>Status</t>
         </is>
       </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>Product ID</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -7512,6 +7517,11 @@
           <t>Active</t>
         </is>
       </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>PRD-041</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -7550,6 +7560,11 @@
           <t>Active</t>
         </is>
       </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>PRD-042</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -7588,6 +7603,11 @@
           <t>Active</t>
         </is>
       </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>PRD-043</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -7626,6 +7646,11 @@
           <t>Active</t>
         </is>
       </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>PRD-044</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -7662,6 +7687,11 @@
       <c r="J6" t="inlineStr">
         <is>
           <t>Active</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>PRD-045</t>
         </is>
       </c>
     </row>
@@ -9945,7 +9975,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10502,6 +10532,33 @@
       <c r="G16" t="inlineStr">
         <is>
           <t>📢</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>CAT-RNT-001</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Rental Equipment</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Rental</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Equipment available for rental</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Product</t>
         </is>
       </c>
     </row>
@@ -10516,7 +10573,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L41"/>
+  <dimension ref="A1:L46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F23" sqref="F23"/>
@@ -12826,6 +12883,246 @@
         <v>0</v>
       </c>
       <c r="L41" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>PRD-041</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>HD Projector</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Rental</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>Product</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>RNT-PRD-PROJ</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>HD projector for presentations and events</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>CAT-RNT-001</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>Rental Equipment</t>
+        </is>
+      </c>
+      <c r="K42" t="n">
+        <v>0</v>
+      </c>
+      <c r="L42" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>PRD-042</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Conference Room AV Kit</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Rental</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>Product</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>RNT-PRD-AV</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>Complete AV kit for conference rooms</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>CAT-RNT-001</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>Rental Equipment</t>
+        </is>
+      </c>
+      <c r="K43" t="n">
+        <v>0</v>
+      </c>
+      <c r="L43" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>PRD-043</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Laptop Rental Unit</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Rental</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>Product</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>RNT-PRD-LAP</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>Laptop available for short-term rental</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>CAT-RNT-001</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>Rental Equipment</t>
+        </is>
+      </c>
+      <c r="K44" t="n">
+        <v>0</v>
+      </c>
+      <c r="L44" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>PRD-044</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Portable PA System</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Rental</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>Product</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>RNT-PRD-PA</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>Portable public address system for events</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>CAT-RNT-001</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>Rental Equipment</t>
+        </is>
+      </c>
+      <c r="K45" t="n">
+        <v>0</v>
+      </c>
+      <c r="L45" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>PRD-045</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Display Monitor (Large)</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Rental</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>Product</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>RNT-PRD-MON</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>Large display monitor for events and trade shows</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>CAT-RNT-001</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>Rental Equipment</t>
+        </is>
+      </c>
+      <c r="K46" t="n">
+        <v>0</v>
+      </c>
+      <c r="L46" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>